<commit_message>
Roughly finish the project using year data
</commit_message>
<xml_diff>
--- a/dataset/year/keys.xlsx
+++ b/dataset/year/keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mscs\visutalization\dataset\year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9F0D0F-CA74-49BA-984C-ACAC2CA1966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164A6056-0B6E-46B1-8E78-A8BEEB6B2DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19A49C19-652D-4839-922F-3D14A1FDA5C0}"/>
   </bookViews>
@@ -863,6 +863,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -880,9 +883,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F10173-0541-443E-A12E-EE5FA9359E2E}">
   <dimension ref="A1:O16393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -1228,7 +1228,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="15.6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1259,7 +1259,7 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="15.6">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="2" t="s">
         <v>116</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="15.6">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="14" t="s">
         <v>106</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.6">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="12" t="s">
         <v>112</v>
       </c>
@@ -1406,13 +1406,13 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" s="6" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1439,7 +1439,7 @@
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15" s="6" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A9" s="17"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="23"/>
       <c r="C9" s="11" t="s">
         <v>42</v>
@@ -1468,7 +1468,7 @@
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" ht="15.6">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="12" t="s">
         <v>119</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" s="6" customFormat="1" ht="31.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="9" t="s">
         <v>93</v>
       </c>
@@ -1548,7 +1548,7 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:15" s="6" customFormat="1" ht="31.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1571,7 +1571,7 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1" ht="15.6">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>100</v>
       </c>
@@ -1604,11 +1604,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.6">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="21" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1625,11 +1625,11 @@
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="15.6">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1647,11 +1647,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.6">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="5" t="s">
         <v>65</v>
       </c>
@@ -1687,7 +1687,7 @@
       <c r="A22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="15.6">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -1709,7 +1709,7 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:11" ht="15.6">
-      <c r="A24" s="18"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="14" t="s">
         <v>108</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:11" ht="15.6">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="14" t="s">
         <v>111</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="15.6">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="14" t="s">
         <v>109</v>
       </c>

</xml_diff>